<commit_message>
Add English app and data update
</commit_message>
<xml_diff>
--- a/DataParkir_Fix.xlsx
+++ b/DataParkir_Fix.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TarifParkirBanyumas\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TarifParkirProgresifBanyumas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C832321-DB60-4165-A319-71C7FF69DBAD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42BCA2DA-0B0C-4098-9548-187333082D07}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-90" yWindow="0" windowWidth="9780" windowHeight="10170" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20" yWindow="740" windowWidth="19180" windowHeight="10060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -38401,16 +38401,10 @@
     <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="4" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="165" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="1" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -38421,12 +38415,18 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -38650,8 +38650,8 @@
   </sheetPr>
   <dimension ref="A1:AO1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="62" workbookViewId="0">
-      <selection activeCell="AN5" sqref="AN5"/>
+    <sheetView tabSelected="1" topLeftCell="Z1" zoomScale="62" workbookViewId="0">
+      <selection activeCell="AF1" sqref="AF1:AI2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -38674,104 +38674,107 @@
     <col min="34" max="34" width="25" customWidth="1"/>
     <col min="35" max="35" width="23.08984375" customWidth="1"/>
     <col min="36" max="36" width="22.7265625" customWidth="1"/>
-    <col min="37" max="41" width="14.08984375" customWidth="1"/>
+    <col min="37" max="37" width="24.81640625" customWidth="1"/>
+    <col min="38" max="38" width="28.1796875" customWidth="1"/>
+    <col min="39" max="39" width="24.90625" customWidth="1"/>
+    <col min="40" max="41" width="14.08984375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:41" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="149" t="s">
+      <c r="A1" s="155" t="s">
         <v>4475</v>
       </c>
-      <c r="B1" s="151" t="s">
+      <c r="B1" s="160" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="151" t="s">
+      <c r="C1" s="160" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="149" t="s">
+      <c r="D1" s="155" t="s">
         <v>4476</v>
       </c>
-      <c r="E1" s="149" t="s">
+      <c r="E1" s="155" t="s">
         <v>4477</v>
       </c>
-      <c r="F1" s="149" t="s">
+      <c r="F1" s="155" t="s">
         <v>4478</v>
       </c>
-      <c r="G1" s="149" t="s">
+      <c r="G1" s="155" t="s">
         <v>4479</v>
       </c>
-      <c r="H1" s="149" t="s">
+      <c r="H1" s="155" t="s">
         <v>4480</v>
       </c>
-      <c r="I1" s="149" t="s">
+      <c r="I1" s="155" t="s">
         <v>4481</v>
       </c>
-      <c r="J1" s="149" t="s">
+      <c r="J1" s="155" t="s">
         <v>4482</v>
       </c>
-      <c r="K1" s="149" t="s">
+      <c r="K1" s="155" t="s">
         <v>4483</v>
       </c>
-      <c r="L1" s="149" t="s">
+      <c r="L1" s="155" t="s">
         <v>4484</v>
       </c>
-      <c r="M1" s="149" t="s">
+      <c r="M1" s="155" t="s">
         <v>4485</v>
       </c>
-      <c r="N1" s="149" t="s">
+      <c r="N1" s="155" t="s">
         <v>4486</v>
       </c>
-      <c r="O1" s="149" t="s">
+      <c r="O1" s="155" t="s">
         <v>4487</v>
       </c>
-      <c r="P1" s="157" t="s">
+      <c r="P1" s="156" t="s">
         <v>4488</v>
       </c>
-      <c r="Q1" s="158"/>
-      <c r="R1" s="158"/>
-      <c r="S1" s="159"/>
-      <c r="T1" s="157" t="s">
+      <c r="Q1" s="157"/>
+      <c r="R1" s="157"/>
+      <c r="S1" s="158"/>
+      <c r="T1" s="156" t="s">
         <v>4493</v>
       </c>
-      <c r="U1" s="158"/>
-      <c r="V1" s="158"/>
-      <c r="W1" s="159"/>
-      <c r="X1" s="160" t="s">
+      <c r="U1" s="157"/>
+      <c r="V1" s="157"/>
+      <c r="W1" s="158"/>
+      <c r="X1" s="159" t="s">
         <v>4494</v>
       </c>
-      <c r="Y1" s="158"/>
-      <c r="Z1" s="158"/>
-      <c r="AA1" s="159"/>
-      <c r="AB1" s="160" t="s">
+      <c r="Y1" s="157"/>
+      <c r="Z1" s="157"/>
+      <c r="AA1" s="158"/>
+      <c r="AB1" s="159" t="s">
         <v>4495</v>
       </c>
-      <c r="AC1" s="158"/>
-      <c r="AD1" s="158"/>
-      <c r="AE1" s="159"/>
-      <c r="AF1" s="152" t="s">
+      <c r="AC1" s="157"/>
+      <c r="AD1" s="157"/>
+      <c r="AE1" s="158"/>
+      <c r="AF1" s="149" t="s">
         <v>4496</v>
       </c>
-      <c r="AG1" s="152" t="s">
+      <c r="AG1" s="149" t="s">
         <v>4497</v>
       </c>
-      <c r="AH1" s="152" t="s">
+      <c r="AH1" s="149" t="s">
         <v>4498</v>
       </c>
-      <c r="AI1" s="152" t="s">
+      <c r="AI1" s="149" t="s">
         <v>4499</v>
       </c>
-      <c r="AJ1" s="155" t="s">
+      <c r="AJ1" s="153" t="s">
         <v>4500</v>
       </c>
-      <c r="AK1" s="155" t="s">
+      <c r="AK1" s="153" t="s">
         <v>4501</v>
       </c>
-      <c r="AL1" s="156" t="s">
+      <c r="AL1" s="154" t="s">
         <v>4502</v>
       </c>
-      <c r="AM1" s="155" t="s">
+      <c r="AM1" s="153" t="s">
         <v>4503</v>
       </c>
-      <c r="AO1" s="153"/>
+      <c r="AO1" s="151"/>
     </row>
     <row r="2" spans="1:41" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="150"/>
@@ -38845,7 +38848,7 @@
       <c r="AK2" s="150"/>
       <c r="AL2" s="150"/>
       <c r="AM2" s="150"/>
-      <c r="AO2" s="154"/>
+      <c r="AO2" s="152"/>
     </row>
     <row r="3" spans="1:41" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
@@ -97611,12 +97614,16 @@
     </row>
   </sheetData>
   <mergeCells count="28">
-    <mergeCell ref="AI1:AI2"/>
-    <mergeCell ref="AO1:AO2"/>
-    <mergeCell ref="AJ1:AJ2"/>
-    <mergeCell ref="AK1:AK2"/>
-    <mergeCell ref="AL1:AL2"/>
-    <mergeCell ref="AM1:AM2"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="E1:E2"/>
+    <mergeCell ref="F1:F2"/>
+    <mergeCell ref="G1:G2"/>
+    <mergeCell ref="H1:H2"/>
+    <mergeCell ref="I1:I2"/>
+    <mergeCell ref="J1:J2"/>
     <mergeCell ref="K1:K2"/>
     <mergeCell ref="L1:L2"/>
     <mergeCell ref="M1:M2"/>
@@ -97629,16 +97636,12 @@
     <mergeCell ref="AB1:AE1"/>
     <mergeCell ref="AF1:AF2"/>
     <mergeCell ref="AG1:AG2"/>
-    <mergeCell ref="F1:F2"/>
-    <mergeCell ref="G1:G2"/>
-    <mergeCell ref="H1:H2"/>
-    <mergeCell ref="I1:I2"/>
-    <mergeCell ref="J1:J2"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="D1:D2"/>
-    <mergeCell ref="E1:E2"/>
+    <mergeCell ref="AI1:AI2"/>
+    <mergeCell ref="AO1:AO2"/>
+    <mergeCell ref="AJ1:AJ2"/>
+    <mergeCell ref="AK1:AK2"/>
+    <mergeCell ref="AL1:AL2"/>
+    <mergeCell ref="AM1:AM2"/>
   </mergeCells>
   <printOptions horizontalCentered="1" gridLines="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>

</xml_diff>